<commit_message>
Updated Stack Creation and WorkPlan
</commit_message>
<xml_diff>
--- a/work-plan.xlsx
+++ b/work-plan.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tr_lnd_user.PACD-516P1DK-D\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="0" windowWidth="27420" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="1245" yWindow="0" windowWidth="19440" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>Tasks</t>
   </si>
@@ -132,81 +127,6 @@
   </si>
   <si>
     <t>1. Set up</t>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF212121"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212121"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Docker compose</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF212121"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212121"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Platform management</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>c.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF212121"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212121"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Docker cartridges</t>
-    </r>
-  </si>
-  <si>
-    <t>4. Document your project</t>
   </si>
   <si>
     <r>
@@ -309,6 +229,42 @@
   </si>
   <si>
     <t xml:space="preserve">3. Creation of Cartridges </t>
+  </si>
+  <si>
+    <t>5. Document your project</t>
+  </si>
+  <si>
+    <t>b. Platform management</t>
+  </si>
+  <si>
+    <t>c. Docker cartridges</t>
+  </si>
+  <si>
+    <t>a. Docker compose</t>
+  </si>
+  <si>
+    <t>a. Gitlab to Jenkins</t>
+  </si>
+  <si>
+    <t>4. Configurations in Jenkins</t>
+  </si>
+  <si>
+    <t>b. Maven to Jenkins</t>
+  </si>
+  <si>
+    <t>c. JUnit to Jenkins</t>
+  </si>
+  <si>
+    <t>d. Sonarqube to Jenkins</t>
+  </si>
+  <si>
+    <t>e. Ansible to Jenkins</t>
+  </si>
+  <si>
+    <t>f. Tomcat to Jenkins</t>
+  </si>
+  <si>
+    <t>g. Selenium to Jenkins</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1358,7 +1314,7 @@
     </row>
     <row r="23" spans="1:15" ht="21.95" customHeight="1">
       <c r="A23" s="33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1405,7 +1361,7 @@
     </row>
     <row r="25" spans="1:15" ht="21.95" customHeight="1">
       <c r="A25" s="34" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1424,7 +1380,7 @@
     </row>
     <row r="26" spans="1:15" ht="21.95" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="14">
@@ -1452,7 +1408,7 @@
     </row>
     <row r="27" spans="1:15" ht="21.95" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="14">
@@ -1480,7 +1436,7 @@
     </row>
     <row r="28" spans="1:15" ht="21.95" customHeight="1">
       <c r="A28" s="36" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="14">
@@ -1508,7 +1464,7 @@
     </row>
     <row r="29" spans="1:15" ht="21.95" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1525,16 +1481,16 @@
       <c r="N29" s="16"/>
       <c r="O29" s="5"/>
     </row>
-    <row r="30" spans="1:15" ht="87" customHeight="1">
-      <c r="A30" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="30"/>
+    <row r="30" spans="1:15" ht="21.95" customHeight="1">
+      <c r="A30" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="4"/>
       <c r="C30" s="14">
-        <v>42627</v>
+        <v>42626</v>
       </c>
       <c r="D30" s="14">
-        <v>42627</v>
+        <v>42626</v>
       </c>
       <c r="E30" s="4">
         <f>D30-C30</f>
@@ -1553,19 +1509,18 @@
       <c r="N30" s="1"/>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15" ht="78.75" customHeight="1">
+    <row r="31" spans="1:15" ht="21.95" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="14">
-        <v>42627</v>
+        <v>42622</v>
       </c>
       <c r="D31" s="14">
-        <v>42627</v>
+        <v>42622</v>
       </c>
       <c r="E31" s="4">
-        <f>D31-C31</f>
         <v>0</v>
       </c>
       <c r="F31" s="11" t="s">
@@ -1581,19 +1536,18 @@
       <c r="N31" s="1"/>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15" ht="72.75" customHeight="1">
+    <row r="32" spans="1:15" ht="21.95" customHeight="1">
       <c r="A32" s="36" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="14">
-        <v>42628</v>
+        <v>42622</v>
       </c>
       <c r="D32" s="14">
-        <v>42628</v>
+        <v>42622</v>
       </c>
       <c r="E32" s="4">
-        <f>D32-C32</f>
         <v>0</v>
       </c>
       <c r="F32" s="11" t="s">
@@ -1609,19 +1563,18 @@
       <c r="N32" s="1"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" ht="61.5" customHeight="1">
+    <row r="33" spans="1:15" ht="21.95" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="14">
-        <v>42628</v>
+        <v>42626</v>
       </c>
       <c r="D33" s="14">
-        <v>42628</v>
+        <v>42626</v>
       </c>
       <c r="E33" s="4">
-        <f>D33-C33</f>
         <v>0</v>
       </c>
       <c r="F33" s="11" t="s">
@@ -1638,51 +1591,263 @@
       <c r="O33" s="4"/>
     </row>
     <row r="34" spans="1:15" ht="21.95" customHeight="1">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="14">
+        <v>42626</v>
+      </c>
+      <c r="D34" s="14">
+        <v>42626</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="1:15" ht="21.95" customHeight="1">
+      <c r="A35" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="14">
+        <v>42622</v>
+      </c>
+      <c r="D35" s="14">
+        <v>42622</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="4"/>
+    </row>
+    <row r="36" spans="1:15" ht="21.95" customHeight="1">
+      <c r="A36" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="14">
+        <v>42626</v>
+      </c>
+      <c r="D36" s="14">
+        <v>42626</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="1:15" ht="21.95" customHeight="1">
+      <c r="A37" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="5"/>
+    </row>
+    <row r="38" spans="1:15" ht="87" customHeight="1">
+      <c r="A38" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="14">
+        <v>42627</v>
+      </c>
+      <c r="D38" s="14">
+        <v>42627</v>
+      </c>
+      <c r="E38" s="4">
+        <f>D38-C38</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="1:15" ht="78.75" customHeight="1">
+      <c r="A39" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="14">
+        <v>42627</v>
+      </c>
+      <c r="D39" s="14">
+        <v>42627</v>
+      </c>
+      <c r="E39" s="4">
+        <f>D39-C39</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="4"/>
+    </row>
+    <row r="40" spans="1:15" ht="72.75" customHeight="1">
+      <c r="A40" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="14">
+        <v>42628</v>
+      </c>
+      <c r="D40" s="14">
+        <v>42628</v>
+      </c>
+      <c r="E40" s="4">
+        <f>D40-C40</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="1:15" ht="61.5" customHeight="1">
+      <c r="A41" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="14">
+        <v>42628</v>
+      </c>
+      <c r="D41" s="14">
+        <v>42628</v>
+      </c>
+      <c r="E41" s="4">
+        <f>D41-C41</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="4"/>
+    </row>
+    <row r="42" spans="1:15" ht="21.95" customHeight="1">
+      <c r="A42" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19">
+      <c r="B42" s="18"/>
+      <c r="C42" s="19">
         <v>42629</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D42" s="19">
         <v>42629</v>
       </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="18"/>
-    </row>
-    <row r="35" spans="1:15" ht="29.1" customHeight="1"/>
-    <row r="39" spans="1:15" ht="18.75">
-      <c r="A39" s="23" t="s">
+      <c r="E42" s="18"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="18"/>
+    </row>
+    <row r="43" spans="1:15" ht="29.1" customHeight="1"/>
+    <row r="47" spans="1:15" ht="18.75">
+      <c r="A47" s="23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="8" t="s">
+    <row r="48" spans="1:15">
+      <c r="A48" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
-      <c r="A41" s="7" t="s">
+    <row r="49" spans="1:1">
+      <c r="A49" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
-      <c r="A42" s="10" t="s">
+    <row r="50" spans="1:1">
+      <c r="A50" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
-      <c r="A43" s="31" t="s">
+    <row r="51" spans="1:1">
+      <c r="A51" s="31" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>